<commit_message>
backlog and burndown chart updated
</commit_message>
<xml_diff>
--- a/docs/sprints/2/Burndown Chart + Sprint Backlog.xlsx
+++ b/docs/sprints/2/Burndown Chart + Sprint Backlog.xlsx
@@ -542,48 +542,48 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -985,28 +985,28 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1572,7 +1572,7 @@
       <pane xSplit="6" ySplit="7" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="N12" sqref="N12"/>
+      <selection pane="bottomRight" activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1591,99 +1591,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="4" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="43" t="s">
+      <c r="B1" s="46"/>
+      <c r="C1" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="41" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="43" t="s">
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="43" t="s">
+      <c r="B2" s="46"/>
+      <c r="C2" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="42" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
       <c r="J2" s="25">
         <v>8</v>
       </c>
       <c r="K2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="43" t="s">
+      <c r="L2" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
     </row>
     <row r="3" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="42" t="s">
+      <c r="A3" s="46"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
       <c r="J3" s="26">
         <v>1</v>
       </c>
-      <c r="K3" s="41" t="s">
+      <c r="K3" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41" t="s">
+      <c r="L3" s="46"/>
+      <c r="M3" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
       <c r="G4" s="27" t="s">
         <v>3</v>
       </c>
@@ -1725,12 +1725,12 @@
       </c>
     </row>
     <row r="5" spans="1:19" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
       <c r="G5" s="28" t="s">
         <v>25</v>
       </c>
@@ -1765,13 +1765,13 @@
     </row>
     <row r="6" spans="1:19" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29"/>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
       <c r="G6" s="30">
         <f>G7</f>
         <v>40</v>
@@ -1827,48 +1827,48 @@
     </row>
     <row r="7" spans="1:19" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33"/>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
       <c r="G7" s="31">
         <f>SUM(G9:G36)</f>
         <v>40</v>
       </c>
       <c r="H7" s="31">
         <f t="shared" ref="H7:O7" si="1">SUM(H9:H36)</f>
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="I7" s="31">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="J7" s="31">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="K7" s="31">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="L7" s="31">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="M7" s="31">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="N7" s="31">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="O7" s="31">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="P7" s="23"/>
       <c r="Q7" s="9"/>
@@ -1877,13 +1877,13 @@
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="34"/>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="49"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="40"/>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
@@ -1902,18 +1902,18 @@
       <c r="A9" s="34">
         <v>1</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="52"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="43"/>
       <c r="G9" s="35">
         <v>8</v>
       </c>
       <c r="H9" s="35">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I9" s="35">
         <v>0</v>
@@ -1945,13 +1945,13 @@
       <c r="A10" s="34">
         <v>2</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="52"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="35">
         <v>8</v>
       </c>
@@ -1959,25 +1959,25 @@
         <v>8</v>
       </c>
       <c r="I10" s="35">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J10" s="35">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K10" s="35">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L10" s="35">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="M10" s="35">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="N10" s="35">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O10" s="35">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="P10" s="24"/>
       <c r="Q10" s="17"/>
@@ -1988,13 +1988,13 @@
       <c r="A11" s="34">
         <v>3</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="52"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="43"/>
       <c r="G11" s="35">
         <v>7</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>7</v>
       </c>
       <c r="O11" s="36">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="P11" s="24"/>
       <c r="Q11" s="17"/>
@@ -2031,13 +2031,13 @@
       <c r="A12" s="34">
         <v>4</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="52"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="43"/>
       <c r="G12" s="35">
         <v>7</v>
       </c>
@@ -2048,22 +2048,22 @@
         <v>7</v>
       </c>
       <c r="J12" s="35">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="K12" s="35">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L12" s="35">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="M12" s="35">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="N12" s="35">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="O12" s="36">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="P12" s="24"/>
       <c r="Q12" s="17"/>
@@ -2074,13 +2074,13 @@
       <c r="A13" s="34">
         <v>5</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
       <c r="G13" s="35">
         <v>10</v>
       </c>
@@ -2103,10 +2103,10 @@
         <v>10</v>
       </c>
       <c r="N13" s="35">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O13" s="36">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P13" s="24"/>
       <c r="Q13" s="17"/>
@@ -2157,11 +2157,11 @@
     </row>
     <row r="16" spans="1:19" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
       <c r="G16" s="21"/>
       <c r="H16" s="21"/>
       <c r="I16" s="21"/>
@@ -2241,11 +2241,11 @@
     </row>
     <row r="20" spans="1:19" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="34"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
       <c r="I20" s="21"/>
@@ -2325,11 +2325,11 @@
     </row>
     <row r="24" spans="1:19" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="34"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
       <c r="G24" s="21"/>
       <c r="H24" s="21"/>
       <c r="I24" s="21"/>
@@ -2409,11 +2409,11 @@
     </row>
     <row r="28" spans="1:19" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="34"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
       <c r="I28" s="21"/>
@@ -2805,37 +2805,6 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F3"/>
-    <mergeCell ref="B4:F5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B20:F20"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="B21:F21"/>
@@ -2844,6 +2813,37 @@
     <mergeCell ref="B25:F25"/>
     <mergeCell ref="B26:F26"/>
     <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F3"/>
+    <mergeCell ref="B4:F5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="G17:O19 G21:O23 G25:O27 G29:O31 G9:O12 G15:O15">
@@ -2865,6 +2865,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Document_x0020_Type xmlns="c0e2046d-6394-4221-b9e6-4c92e93e9cfa">1 - Planning</Document_x0020_Type>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3D38A84C2BDA643A4CDF6700786B38C" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="72d71d1fa8fd145f6328292242f562f6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c0e2046d-6394-4221-b9e6-4c92e93e9cfa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d131b300f296c1bc07c44b8d961fd912" ns2:_="">
     <xsd:import namespace="c0e2046d-6394-4221-b9e6-4c92e93e9cfa"/>
@@ -2931,24 +2948,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFDF09ED-BC2B-42F3-BD94-84AC894813D6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="c0e2046d-6394-4221-b9e6-4c92e93e9cfa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Document_x0020_Type xmlns="c0e2046d-6394-4221-b9e6-4c92e93e9cfa">1 - Planning</Document_x0020_Type>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B083C5B-91DA-4961-965C-4DCFA43B4D69}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF673A54-9E2F-4DC5-957C-747EA2C9F553}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2963,28 +2987,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B083C5B-91DA-4961-965C-4DCFA43B4D69}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFDF09ED-BC2B-42F3-BD94-84AC894813D6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="c0e2046d-6394-4221-b9e6-4c92e93e9cfa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>